<commit_message>
Update results from parameter search
</commit_message>
<xml_diff>
--- a/Results/aggregated_results.xlsx
+++ b/Results/aggregated_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
   <si>
     <t>optimiser</t>
   </si>
@@ -449,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W80"/>
+  <dimension ref="A1:W82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4729,61 +4729,61 @@
         <v>0.25</v>
       </c>
       <c r="E61">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F61">
-        <v>0.42049</v>
+        <v>0.41859</v>
       </c>
       <c r="G61">
-        <v>0.01381</v>
+        <v>0.01537</v>
       </c>
       <c r="H61">
-        <v>1223.428</v>
+        <v>1314.836</v>
       </c>
       <c r="I61">
-        <v>529.09419</v>
+        <v>504.03407</v>
       </c>
       <c r="J61">
-        <v>271.406</v>
+        <v>291.926</v>
       </c>
       <c r="K61">
-        <v>118.66427</v>
+        <v>113.06308</v>
       </c>
       <c r="L61">
-        <v>0.86953</v>
+        <v>0.87157</v>
       </c>
       <c r="M61">
-        <v>0.01427</v>
+        <v>0.01046</v>
       </c>
       <c r="N61">
-        <v>186</v>
+        <v>185.7</v>
       </c>
       <c r="O61">
-        <v>5.33854</v>
+        <v>5.37587</v>
       </c>
       <c r="P61">
-        <v>41</v>
+        <v>41.3</v>
       </c>
       <c r="Q61">
-        <v>5.33854</v>
+        <v>5.37587</v>
       </c>
       <c r="R61">
-        <v>22.8</v>
+        <v>21.5</v>
       </c>
       <c r="S61">
-        <v>3.96232</v>
+        <v>4.64878</v>
       </c>
       <c r="T61">
-        <v>239.2</v>
+        <v>240.5</v>
       </c>
       <c r="U61">
-        <v>3.96232</v>
+        <v>4.64878</v>
       </c>
       <c r="V61">
-        <v>0.88235</v>
+        <v>0.88451</v>
       </c>
       <c r="W61">
-        <v>0.01258</v>
+        <v>0.009310000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:23">
@@ -5084,61 +5084,61 @@
         <v>0.2</v>
       </c>
       <c r="E66">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F66">
-        <v>0.44706</v>
+        <v>0.44274</v>
       </c>
       <c r="G66">
-        <v>0.04597</v>
+        <v>0.05049</v>
       </c>
       <c r="H66">
-        <v>1686.95714</v>
+        <v>1564.504</v>
       </c>
       <c r="I66">
-        <v>519.87212</v>
+        <v>549.01656</v>
       </c>
       <c r="J66">
-        <v>339.39857</v>
+        <v>314.439</v>
       </c>
       <c r="K66">
-        <v>105.82302</v>
+        <v>111.75621</v>
       </c>
       <c r="L66">
-        <v>0.84779</v>
+        <v>0.85031</v>
       </c>
       <c r="M66">
-        <v>0.01125</v>
+        <v>0.01215</v>
       </c>
       <c r="N66">
-        <v>179.42857</v>
+        <v>180.4</v>
       </c>
       <c r="O66">
-        <v>5.15937</v>
+        <v>5.96657</v>
       </c>
       <c r="P66">
-        <v>47.57143</v>
+        <v>46.6</v>
       </c>
       <c r="Q66">
-        <v>5.15937</v>
+        <v>5.96657</v>
       </c>
       <c r="R66">
-        <v>26.85714</v>
+        <v>26.6</v>
       </c>
       <c r="S66">
-        <v>6.4402</v>
+        <v>6.6366</v>
       </c>
       <c r="T66">
-        <v>235.14286</v>
+        <v>235.4</v>
       </c>
       <c r="U66">
-        <v>6.4402</v>
+        <v>6.6366</v>
       </c>
       <c r="V66">
-        <v>0.86328</v>
+        <v>0.86537</v>
       </c>
       <c r="W66">
-        <v>0.0111</v>
+        <v>0.01157</v>
       </c>
     </row>
     <row r="67" spans="1:23">
@@ -5362,67 +5362,67 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="D70">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E70">
         <v>10</v>
       </c>
       <c r="F70">
-        <v>0.16432</v>
+        <v>0.20612</v>
       </c>
       <c r="G70">
-        <v>0.02382</v>
+        <v>0.03054</v>
       </c>
       <c r="H70">
-        <v>433.043</v>
+        <v>1215.185</v>
       </c>
       <c r="I70">
-        <v>201.02224</v>
+        <v>575.73763</v>
       </c>
       <c r="J70">
-        <v>86.84999999999999</v>
+        <v>243.807</v>
       </c>
       <c r="K70">
-        <v>40.78146</v>
+        <v>116.91754</v>
       </c>
       <c r="L70">
-        <v>0.93497</v>
+        <v>0.9222900000000001</v>
       </c>
       <c r="M70">
-        <v>0.01156</v>
+        <v>0.01268</v>
       </c>
       <c r="N70">
-        <v>208.2</v>
+        <v>204.4</v>
       </c>
       <c r="O70">
-        <v>4.6619</v>
+        <v>5.85377</v>
       </c>
       <c r="P70">
-        <v>18.8</v>
+        <v>22.6</v>
       </c>
       <c r="Q70">
-        <v>4.6619</v>
+        <v>5.85377</v>
       </c>
       <c r="R70">
-        <v>13</v>
+        <v>15.4</v>
       </c>
       <c r="S70">
-        <v>4.10961</v>
+        <v>3.20416</v>
       </c>
       <c r="T70">
-        <v>249</v>
+        <v>246.6</v>
       </c>
       <c r="U70">
-        <v>4.10961</v>
+        <v>3.20416</v>
       </c>
       <c r="V70">
-        <v>0.93998</v>
+        <v>0.92853</v>
       </c>
       <c r="W70">
-        <v>0.01054</v>
+        <v>0.01115</v>
       </c>
     </row>
     <row r="71" spans="1:23">
@@ -5436,64 +5436,64 @@
         <v>0.005</v>
       </c>
       <c r="D71">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E71">
         <v>10</v>
       </c>
       <c r="F71">
-        <v>0.16406</v>
+        <v>0.16432</v>
       </c>
       <c r="G71">
-        <v>0.02951</v>
+        <v>0.02382</v>
       </c>
       <c r="H71">
-        <v>514.636</v>
+        <v>433.043</v>
       </c>
       <c r="I71">
-        <v>258.40812</v>
+        <v>201.02224</v>
       </c>
       <c r="J71">
-        <v>103.279</v>
+        <v>86.84999999999999</v>
       </c>
       <c r="K71">
-        <v>52.40384</v>
+        <v>40.78146</v>
       </c>
       <c r="L71">
-        <v>0.93599</v>
+        <v>0.93497</v>
       </c>
       <c r="M71">
-        <v>0.01374</v>
+        <v>0.01156</v>
       </c>
       <c r="N71">
-        <v>208.3</v>
+        <v>208.2</v>
       </c>
       <c r="O71">
-        <v>5.37587</v>
+        <v>4.6619</v>
       </c>
       <c r="P71">
-        <v>18.7</v>
+        <v>18.8</v>
       </c>
       <c r="Q71">
-        <v>5.37587</v>
+        <v>4.6619</v>
       </c>
       <c r="R71">
-        <v>12.6</v>
+        <v>13</v>
       </c>
       <c r="S71">
-        <v>3.74759</v>
+        <v>4.10961</v>
       </c>
       <c r="T71">
-        <v>249.4</v>
+        <v>249</v>
       </c>
       <c r="U71">
-        <v>3.74759</v>
+        <v>4.10961</v>
       </c>
       <c r="V71">
-        <v>0.94099</v>
+        <v>0.93998</v>
       </c>
       <c r="W71">
-        <v>0.01246</v>
+        <v>0.01054</v>
       </c>
     </row>
     <row r="72" spans="1:23">
@@ -5507,64 +5507,64 @@
         <v>0.005</v>
       </c>
       <c r="D72">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="E72">
         <v>10</v>
       </c>
       <c r="F72">
-        <v>0.16294</v>
+        <v>0.16406</v>
       </c>
       <c r="G72">
-        <v>0.02397</v>
+        <v>0.02951</v>
       </c>
       <c r="H72">
-        <v>440.737</v>
+        <v>514.636</v>
       </c>
       <c r="I72">
-        <v>230.22491</v>
+        <v>258.40812</v>
       </c>
       <c r="J72">
-        <v>88.34099999999999</v>
+        <v>103.279</v>
       </c>
       <c r="K72">
-        <v>46.65735</v>
+        <v>52.40384</v>
       </c>
       <c r="L72">
-        <v>0.93701</v>
+        <v>0.93599</v>
       </c>
       <c r="M72">
-        <v>0.01019</v>
+        <v>0.01374</v>
       </c>
       <c r="N72">
-        <v>209.2</v>
+        <v>208.3</v>
       </c>
       <c r="O72">
-        <v>4.15799</v>
+        <v>5.37587</v>
       </c>
       <c r="P72">
-        <v>17.8</v>
+        <v>18.7</v>
       </c>
       <c r="Q72">
-        <v>4.15799</v>
+        <v>5.37587</v>
       </c>
       <c r="R72">
-        <v>13</v>
+        <v>12.6</v>
       </c>
       <c r="S72">
-        <v>3.65148</v>
+        <v>3.74759</v>
       </c>
       <c r="T72">
-        <v>249</v>
+        <v>249.4</v>
       </c>
       <c r="U72">
-        <v>3.65148</v>
+        <v>3.74759</v>
       </c>
       <c r="V72">
-        <v>0.94176</v>
+        <v>0.94099</v>
       </c>
       <c r="W72">
-        <v>0.00936</v>
+        <v>0.01246</v>
       </c>
     </row>
     <row r="73" spans="1:23">
@@ -5572,70 +5572,70 @@
         <v>25</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73">
-        <v>0.0001</v>
+        <v>0.005</v>
       </c>
       <c r="D73">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E73">
         <v>10</v>
       </c>
       <c r="F73">
-        <v>0.27506</v>
+        <v>0.16294</v>
       </c>
       <c r="G73">
-        <v>0.03907</v>
+        <v>0.02397</v>
       </c>
       <c r="H73">
-        <v>1493.626</v>
+        <v>440.737</v>
       </c>
       <c r="I73">
-        <v>605.1402</v>
+        <v>230.22491</v>
       </c>
       <c r="J73">
-        <v>271.209</v>
+        <v>88.34099999999999</v>
       </c>
       <c r="K73">
-        <v>111.938</v>
+        <v>46.65735</v>
       </c>
       <c r="L73">
-        <v>0.89877</v>
+        <v>0.93701</v>
       </c>
       <c r="M73">
-        <v>0.02195</v>
+        <v>0.01019</v>
       </c>
       <c r="N73">
-        <v>196.8</v>
+        <v>209.2</v>
       </c>
       <c r="O73">
-        <v>10.88118</v>
+        <v>4.15799</v>
       </c>
       <c r="P73">
-        <v>30.2</v>
+        <v>17.8</v>
       </c>
       <c r="Q73">
-        <v>10.88118</v>
+        <v>4.15799</v>
       </c>
       <c r="R73">
-        <v>19.3</v>
+        <v>13</v>
       </c>
       <c r="S73">
-        <v>4.66786</v>
+        <v>3.65148</v>
       </c>
       <c r="T73">
-        <v>242.7</v>
+        <v>249</v>
       </c>
       <c r="U73">
-        <v>4.66786</v>
+        <v>3.65148</v>
       </c>
       <c r="V73">
-        <v>0.9077</v>
+        <v>0.94176</v>
       </c>
       <c r="W73">
-        <v>0.01815</v>
+        <v>0.00936</v>
       </c>
     </row>
     <row r="74" spans="1:23">
@@ -5649,64 +5649,64 @@
         <v>0.0001</v>
       </c>
       <c r="D74">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E74">
         <v>10</v>
       </c>
       <c r="F74">
-        <v>0.2967</v>
+        <v>0.27506</v>
       </c>
       <c r="G74">
-        <v>0.04909</v>
+        <v>0.03907</v>
       </c>
       <c r="H74">
-        <v>1494.104</v>
+        <v>1493.626</v>
       </c>
       <c r="I74">
-        <v>604.76877</v>
+        <v>605.1402</v>
       </c>
       <c r="J74">
-        <v>271.343</v>
+        <v>271.209</v>
       </c>
       <c r="K74">
-        <v>111.82804</v>
+        <v>111.938</v>
       </c>
       <c r="L74">
-        <v>0.88139</v>
+        <v>0.89877</v>
       </c>
       <c r="M74">
-        <v>0.02971</v>
+        <v>0.02195</v>
       </c>
       <c r="N74">
-        <v>187.4</v>
+        <v>196.8</v>
       </c>
       <c r="O74">
-        <v>16.47355</v>
+        <v>10.88118</v>
       </c>
       <c r="P74">
-        <v>39.6</v>
+        <v>30.2</v>
       </c>
       <c r="Q74">
-        <v>16.47355</v>
+        <v>10.88118</v>
       </c>
       <c r="R74">
-        <v>18.4</v>
+        <v>19.3</v>
       </c>
       <c r="S74">
-        <v>4.71876</v>
+        <v>4.66786</v>
       </c>
       <c r="T74">
-        <v>243.6</v>
+        <v>242.7</v>
       </c>
       <c r="U74">
-        <v>4.71876</v>
+        <v>4.66786</v>
       </c>
       <c r="V74">
-        <v>0.89424</v>
+        <v>0.9077</v>
       </c>
       <c r="W74">
-        <v>0.02318</v>
+        <v>0.01815</v>
       </c>
     </row>
     <row r="75" spans="1:23">
@@ -5720,64 +5720,64 @@
         <v>0.0001</v>
       </c>
       <c r="D75">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="E75">
         <v>10</v>
       </c>
       <c r="F75">
-        <v>0.2578</v>
+        <v>0.2967</v>
       </c>
       <c r="G75">
-        <v>0.03997</v>
+        <v>0.04909</v>
       </c>
       <c r="H75">
-        <v>1609.69</v>
+        <v>1494.104</v>
       </c>
       <c r="I75">
-        <v>613.8164</v>
+        <v>604.76877</v>
       </c>
       <c r="J75">
-        <v>292.497</v>
+        <v>271.343</v>
       </c>
       <c r="K75">
-        <v>113.30462</v>
+        <v>111.82804</v>
       </c>
       <c r="L75">
-        <v>0.90798</v>
+        <v>0.88139</v>
       </c>
       <c r="M75">
-        <v>0.02065</v>
+        <v>0.02971</v>
       </c>
       <c r="N75">
-        <v>199.6</v>
+        <v>187.4</v>
       </c>
       <c r="O75">
-        <v>10.51137</v>
+        <v>16.47355</v>
       </c>
       <c r="P75">
-        <v>27.4</v>
+        <v>39.6</v>
       </c>
       <c r="Q75">
-        <v>10.51137</v>
+        <v>16.47355</v>
       </c>
       <c r="R75">
-        <v>17.6</v>
+        <v>18.4</v>
       </c>
       <c r="S75">
-        <v>4.22164</v>
+        <v>4.71876</v>
       </c>
       <c r="T75">
-        <v>244.4</v>
+        <v>243.6</v>
       </c>
       <c r="U75">
-        <v>4.22164</v>
+        <v>4.71876</v>
       </c>
       <c r="V75">
-        <v>0.91594</v>
+        <v>0.89424</v>
       </c>
       <c r="W75">
-        <v>0.01715</v>
+        <v>0.02318</v>
       </c>
     </row>
     <row r="76" spans="1:23">
@@ -5788,67 +5788,67 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>0.0005</v>
+        <v>0.0001</v>
       </c>
       <c r="D76">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E76">
         <v>10</v>
       </c>
       <c r="F76">
-        <v>0.18421</v>
+        <v>0.2578</v>
       </c>
       <c r="G76">
-        <v>0.04176</v>
+        <v>0.03997</v>
       </c>
       <c r="H76">
-        <v>1137.868</v>
+        <v>1609.69</v>
       </c>
       <c r="I76">
-        <v>587.95397</v>
+        <v>613.8164</v>
       </c>
       <c r="J76">
-        <v>206.651</v>
+        <v>292.497</v>
       </c>
       <c r="K76">
-        <v>108.07743</v>
+        <v>113.30462</v>
       </c>
       <c r="L76">
-        <v>0.93231</v>
+        <v>0.90798</v>
       </c>
       <c r="M76">
-        <v>0.01507</v>
+        <v>0.02065</v>
       </c>
       <c r="N76">
-        <v>206.1</v>
+        <v>199.6</v>
       </c>
       <c r="O76">
-        <v>6.26188</v>
+        <v>10.51137</v>
       </c>
       <c r="P76">
-        <v>20.9</v>
+        <v>27.4</v>
       </c>
       <c r="Q76">
-        <v>6.26188</v>
+        <v>10.51137</v>
       </c>
       <c r="R76">
-        <v>12.2</v>
+        <v>17.6</v>
       </c>
       <c r="S76">
-        <v>3.8239</v>
+        <v>4.22164</v>
       </c>
       <c r="T76">
-        <v>249.8</v>
+        <v>244.4</v>
       </c>
       <c r="U76">
-        <v>3.8239</v>
+        <v>4.22164</v>
       </c>
       <c r="V76">
-        <v>0.93793</v>
+        <v>0.91594</v>
       </c>
       <c r="W76">
-        <v>0.01346</v>
+        <v>0.01715</v>
       </c>
     </row>
     <row r="77" spans="1:23">
@@ -5862,64 +5862,64 @@
         <v>0.0005</v>
       </c>
       <c r="D77">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E77">
         <v>10</v>
       </c>
       <c r="F77">
-        <v>0.1774</v>
+        <v>0.18421</v>
       </c>
       <c r="G77">
-        <v>0.04022</v>
+        <v>0.04176</v>
       </c>
       <c r="H77">
-        <v>1306.015</v>
+        <v>1137.868</v>
       </c>
       <c r="I77">
-        <v>524.60226</v>
+        <v>587.95397</v>
       </c>
       <c r="J77">
-        <v>237.411</v>
+        <v>206.651</v>
       </c>
       <c r="K77">
-        <v>96.74879</v>
+        <v>108.07743</v>
       </c>
       <c r="L77">
-        <v>0.9366100000000001</v>
+        <v>0.93231</v>
       </c>
       <c r="M77">
-        <v>0.01681</v>
+        <v>0.01507</v>
       </c>
       <c r="N77">
-        <v>207.3</v>
+        <v>206.1</v>
       </c>
       <c r="O77">
-        <v>5.85093</v>
+        <v>6.26188</v>
       </c>
       <c r="P77">
-        <v>19.7</v>
+        <v>20.9</v>
       </c>
       <c r="Q77">
-        <v>5.85093</v>
+        <v>6.26188</v>
       </c>
       <c r="R77">
-        <v>11.3</v>
+        <v>12.2</v>
       </c>
       <c r="S77">
-        <v>3.59166</v>
+        <v>3.8239</v>
       </c>
       <c r="T77">
-        <v>250.7</v>
+        <v>249.8</v>
       </c>
       <c r="U77">
-        <v>3.59166</v>
+        <v>3.8239</v>
       </c>
       <c r="V77">
-        <v>0.9418299999999999</v>
+        <v>0.93793</v>
       </c>
       <c r="W77">
-        <v>0.01508</v>
+        <v>0.01346</v>
       </c>
     </row>
     <row r="78" spans="1:23">
@@ -5930,67 +5930,67 @@
         <v>2</v>
       </c>
       <c r="C78">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="D78">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E78">
         <v>10</v>
       </c>
       <c r="F78">
-        <v>0.15741</v>
+        <v>0.1774</v>
       </c>
       <c r="G78">
-        <v>0.02762</v>
+        <v>0.04022</v>
       </c>
       <c r="H78">
-        <v>348.918</v>
+        <v>1306.015</v>
       </c>
       <c r="I78">
-        <v>139.77743</v>
+        <v>524.60226</v>
       </c>
       <c r="J78">
-        <v>63.241</v>
+        <v>237.411</v>
       </c>
       <c r="K78">
-        <v>25.83873</v>
+        <v>96.74879</v>
       </c>
       <c r="L78">
-        <v>0.93906</v>
+        <v>0.9366100000000001</v>
       </c>
       <c r="M78">
-        <v>0.01184</v>
+        <v>0.01681</v>
       </c>
       <c r="N78">
-        <v>208.5</v>
+        <v>207.3</v>
       </c>
       <c r="O78">
-        <v>4.74342</v>
+        <v>5.85093</v>
       </c>
       <c r="P78">
-        <v>18.5</v>
+        <v>19.7</v>
       </c>
       <c r="Q78">
-        <v>4.74342</v>
+        <v>5.85093</v>
       </c>
       <c r="R78">
         <v>11.3</v>
       </c>
       <c r="S78">
-        <v>3.83116</v>
+        <v>3.59166</v>
       </c>
       <c r="T78">
         <v>250.7</v>
       </c>
       <c r="U78">
-        <v>3.83116</v>
+        <v>3.59166</v>
       </c>
       <c r="V78">
-        <v>0.94392</v>
+        <v>0.9418299999999999</v>
       </c>
       <c r="W78">
-        <v>0.01074</v>
+        <v>0.01508</v>
       </c>
     </row>
     <row r="79" spans="1:23">
@@ -6001,67 +6001,67 @@
         <v>2</v>
       </c>
       <c r="C79">
-        <v>0.005</v>
+        <v>0.0005</v>
       </c>
       <c r="D79">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E79">
         <v>10</v>
       </c>
       <c r="F79">
-        <v>0.15385</v>
+        <v>0.18661</v>
       </c>
       <c r="G79">
-        <v>0.02364</v>
+        <v>0.02877</v>
       </c>
       <c r="H79">
-        <v>376.865</v>
+        <v>1144.936</v>
       </c>
       <c r="I79">
-        <v>146.37892</v>
+        <v>751.55887</v>
       </c>
       <c r="J79">
-        <v>68.486</v>
+        <v>208.161</v>
       </c>
       <c r="K79">
-        <v>27.00646</v>
+        <v>138.08879</v>
       </c>
       <c r="L79">
-        <v>0.93988</v>
+        <v>0.93333</v>
       </c>
       <c r="M79">
-        <v>0.01162</v>
+        <v>0.01007</v>
       </c>
       <c r="N79">
-        <v>209.8</v>
+        <v>206.4</v>
       </c>
       <c r="O79">
-        <v>4.28952</v>
+        <v>4.85798</v>
       </c>
       <c r="P79">
-        <v>17.2</v>
+        <v>20.6</v>
       </c>
       <c r="Q79">
-        <v>4.28952</v>
+        <v>4.85798</v>
       </c>
       <c r="R79">
-        <v>12.2</v>
+        <v>12</v>
       </c>
       <c r="S79">
-        <v>3.48967</v>
+        <v>2.94392</v>
       </c>
       <c r="T79">
-        <v>249.8</v>
+        <v>250</v>
       </c>
       <c r="U79">
-        <v>3.48967</v>
+        <v>2.94392</v>
       </c>
       <c r="V79">
-        <v>0.9444399999999999</v>
+        <v>0.9388300000000001</v>
       </c>
       <c r="W79">
-        <v>0.01061</v>
+        <v>0.00894</v>
       </c>
     </row>
     <row r="80" spans="1:23">
@@ -6075,63 +6075,205 @@
         <v>0.005</v>
       </c>
       <c r="D80">
+        <v>0.15</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
+      <c r="F80">
+        <v>0.15741</v>
+      </c>
+      <c r="G80">
+        <v>0.02762</v>
+      </c>
+      <c r="H80">
+        <v>348.918</v>
+      </c>
+      <c r="I80">
+        <v>139.77743</v>
+      </c>
+      <c r="J80">
+        <v>63.241</v>
+      </c>
+      <c r="K80">
+        <v>25.83873</v>
+      </c>
+      <c r="L80">
+        <v>0.93906</v>
+      </c>
+      <c r="M80">
+        <v>0.01184</v>
+      </c>
+      <c r="N80">
+        <v>208.5</v>
+      </c>
+      <c r="O80">
+        <v>4.74342</v>
+      </c>
+      <c r="P80">
+        <v>18.5</v>
+      </c>
+      <c r="Q80">
+        <v>4.74342</v>
+      </c>
+      <c r="R80">
+        <v>11.3</v>
+      </c>
+      <c r="S80">
+        <v>3.83116</v>
+      </c>
+      <c r="T80">
+        <v>250.7</v>
+      </c>
+      <c r="U80">
+        <v>3.83116</v>
+      </c>
+      <c r="V80">
+        <v>0.94392</v>
+      </c>
+      <c r="W80">
+        <v>0.01074</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
+      <c r="A81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>0.005</v>
+      </c>
+      <c r="D81">
+        <v>0.2</v>
+      </c>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="F81">
+        <v>0.15385</v>
+      </c>
+      <c r="G81">
+        <v>0.02364</v>
+      </c>
+      <c r="H81">
+        <v>376.865</v>
+      </c>
+      <c r="I81">
+        <v>146.37892</v>
+      </c>
+      <c r="J81">
+        <v>68.486</v>
+      </c>
+      <c r="K81">
+        <v>27.00646</v>
+      </c>
+      <c r="L81">
+        <v>0.93988</v>
+      </c>
+      <c r="M81">
+        <v>0.01162</v>
+      </c>
+      <c r="N81">
+        <v>209.8</v>
+      </c>
+      <c r="O81">
+        <v>4.28952</v>
+      </c>
+      <c r="P81">
+        <v>17.2</v>
+      </c>
+      <c r="Q81">
+        <v>4.28952</v>
+      </c>
+      <c r="R81">
+        <v>12.2</v>
+      </c>
+      <c r="S81">
+        <v>3.48967</v>
+      </c>
+      <c r="T81">
+        <v>249.8</v>
+      </c>
+      <c r="U81">
+        <v>3.48967</v>
+      </c>
+      <c r="V81">
+        <v>0.9444399999999999</v>
+      </c>
+      <c r="W81">
+        <v>0.01061</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
+      <c r="A82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>0.005</v>
+      </c>
+      <c r="D82">
         <v>0.25</v>
       </c>
-      <c r="E80">
-        <v>10</v>
-      </c>
-      <c r="F80">
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="F82">
         <v>0.16111</v>
       </c>
-      <c r="G80">
+      <c r="G82">
         <v>0.03213</v>
       </c>
-      <c r="H80">
+      <c r="H82">
         <v>315.344</v>
       </c>
-      <c r="I80">
+      <c r="I82">
         <v>194.10036</v>
       </c>
-      <c r="J80">
+      <c r="J82">
         <v>57.12</v>
       </c>
-      <c r="K80">
+      <c r="K82">
         <v>35.67829</v>
       </c>
-      <c r="L80">
+      <c r="L82">
         <v>0.93865</v>
       </c>
-      <c r="M80">
+      <c r="M82">
         <v>0.01227</v>
       </c>
-      <c r="N80">
+      <c r="N82">
         <v>209.8</v>
       </c>
-      <c r="O80">
+      <c r="O82">
         <v>4.26354</v>
       </c>
-      <c r="P80">
+      <c r="P82">
         <v>17.2</v>
       </c>
-      <c r="Q80">
+      <c r="Q82">
         <v>4.26354</v>
       </c>
-      <c r="R80">
+      <c r="R82">
         <v>12.8</v>
       </c>
-      <c r="S80">
+      <c r="S82">
         <v>3.04777</v>
       </c>
-      <c r="T80">
+      <c r="T82">
         <v>249.2</v>
       </c>
-      <c r="U80">
+      <c r="U82">
         <v>3.04777</v>
       </c>
-      <c r="V80">
+      <c r="V82">
         <v>0.94325</v>
       </c>
-      <c r="W80">
+      <c r="W82">
         <v>0.01114</v>
       </c>
     </row>

</xml_diff>